<commit_message>
updated some aspects of base file by correcting livestock elasticities and new transitions for El Salvador and Jamaica in external file. Regenerated templates with Silvopasture prevalence at 10% instead of 30%
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/sisepuede/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930DC417-8CD6-A645-BF0C-ED76BE2295F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C48743-7F55-AC4B-9FD3-86F09EA7D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21040" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="21040" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -2576,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A631" workbookViewId="0">
-      <selection activeCell="O655" sqref="O655"/>
+    <sheetView tabSelected="1" topLeftCell="W384" workbookViewId="0">
+      <selection activeCell="AD414" sqref="AD414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added individual elasticities of lvst for categories that were missing to fake_data_complete.csv
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/sisepuede/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F6245F-DDEB-074A-866B-342CDB4F90D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89393EB-6874-A646-B4A6-DDC6B9303E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="21040" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:AS680"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A396" workbookViewId="0">
-      <selection activeCell="G406" sqref="G406"/>
+      <selection activeCell="D418" sqref="D418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
continued to replace build_varlist with build_variable_fields
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_af_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_af_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/sisepuede/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89393EB-6874-A646-B4A6-DDC6B9303E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE44E682-F6A7-EB43-9EE3-5E542285758E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="21040" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="500" windowWidth="21040" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:AS680"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A396" workbookViewId="0">
-      <selection activeCell="D418" sqref="D418"/>
+      <selection activeCell="R403" sqref="R403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>